<commit_message>
Saved metadata to irm file
</commit_message>
<xml_diff>
--- a/Matrix resulst.xlsx
+++ b/Matrix resulst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\OneDrive\Documents\Slovenija\Kemijski Institut\Code\Image Alignment\LUMICKS_image_alignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C3D4B6-7308-417A-864B-EECF707F14B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F1764A-4412-46F6-B7A2-E8F8ADF0CC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B30B8E75-9D0C-40B1-88F6-E17F8DA1D242}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>